<commit_message>
Deep Learning with LSTM model
</commit_message>
<xml_diff>
--- a/data/hist_Ratios/MoneyControl/HR_hindustanunilever_using_MoneyControl.xlsx
+++ b/data/hist_Ratios/MoneyControl/HR_hindustanunilever_using_MoneyControl.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,10 +446,15 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Book Value [ExclRevalReserve]/Share (Rs.)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Total Debt/Equity (X)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Price/BV (X)</t>
         </is>
@@ -468,10 +473,15 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>213.71</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>11.97</t>
         </is>
@@ -490,10 +500,15 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>207.49</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>9.87</t>
         </is>
@@ -512,10 +527,15 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>201.85</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>12.04</t>
         </is>
@@ -534,10 +554,15 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>37.18</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>61.81</t>
         </is>
@@ -556,10 +581,15 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>35.46</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>48.16</t>
         </is>
@@ -578,10 +608,15 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>32.75</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>40.79</t>
         </is>
@@ -600,10 +635,15 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>30.05</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>30.28</t>
         </is>
@@ -622,10 +662,15 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>29.07</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>29.91</t>
         </is>
@@ -644,10 +689,15 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>17.21</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>50.71</t>
         </is>
@@ -666,10 +716,15 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>15.15</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>39.85</t>
         </is>
@@ -688,10 +743,15 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>12.36</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>37.70</t>
         </is>
@@ -710,10 +770,15 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>16.25</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>25.23</t>
         </is>
@@ -732,10 +797,15 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>12.31</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>23.12</t>
         </is>
@@ -754,10 +824,15 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>11.84</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>20.16</t>
         </is>
@@ -776,10 +851,15 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>9.45</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>0.20</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>25.20</t>
         </is>
@@ -798,10 +878,15 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>6.61</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>0.06</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>32.38</t>
         </is>
@@ -820,10 +905,15 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>12.34</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>0.03</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>17.55</t>
         </is>
@@ -842,10 +932,15 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>10.47</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>0.02</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>18.84</t>
         </is>
@@ -864,10 +959,15 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>9.50</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>0.70</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>15.10</t>
         </is>

</xml_diff>